<commit_message>
double check f/m info on gerson 2014a
</commit_message>
<xml_diff>
--- a/analysis/formatted_data/xlsx/gerson2014a_cd.xlsx
+++ b/analysis/formatted_data/xlsx/gerson2014a_cd.xlsx
@@ -5,19 +5,19 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shariliu/Dropbox (MIT)/Research/Studies/3Meta/analysis/formatted_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shariliu/Dropbox (MIT)/Research/Studies/3Meta/analysis/formatted_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85D9250-226C-6C4A-AFD8-3F842219D15C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E0F674-F0C2-4D45-BFA6-ADABB5AEB6FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="460" windowWidth="30820" windowHeight="18980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17260" yWindow="460" windowWidth="30820" windowHeight="18980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment Questions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>